<commit_message>
Stable version with clear r cmd check
</commit_message>
<xml_diff>
--- a/data-raw/data structure.xlsx
+++ b/data-raw/data structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s87ja\Dropbox\Work\toXcel\FARS\rfars\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FE4DA331-863C-4167-A5B3-58201208B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE5C8BE-F97D-4905-BC00-DB8CD4A9F214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F622A617-15FC-4761-9D07-38FE22F3629A}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11175" xr2:uid="{F622A617-15FC-4761-9D07-38FE22F3629A}"/>
   </bookViews>
   <sheets>
     <sheet name="data structure" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Steve Jackson</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{AC07BDA0-4064-45EB-A055-21FEDD5BE112}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Jackson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+prep_fars_yyyy should account for new data tables in year year_created-1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
@@ -153,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,19 +195,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -200,16 +248,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -218,6 +273,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFA7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -574,12 +634,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADA2E17-6DE9-4769-B041-028ED6230584}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADA2E17-6DE9-4769-B041-028ED6230584}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +669,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -623,7 +683,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -637,31 +697,31 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>2010</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
+      <c r="A5" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1975</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -679,28 +739,28 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
+      <c r="A7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D7">
-        <v>2014</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>2010</v>
@@ -708,41 +768,41 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2010</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2020</v>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2010</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+      <c r="A11" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>2010</v>
@@ -750,27 +810,30 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>2010</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>2010</v>
@@ -778,238 +841,234 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2019</v>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2010</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D23" s="6">
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D26" s="6">
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2010</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
         <v>2020</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="B28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6">
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="B29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6">
         <v>2020</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
-    <sortCondition descending="1" ref="B2:B29"/>
-    <sortCondition ref="C2:C29"/>
     <sortCondition ref="D2:D29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now using sas files. Other subtle improvements to functionality. Now includes 2015.
</commit_message>
<xml_diff>
--- a/data-raw/data structure.xlsx
+++ b/data-raw/data structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s87ja\Dropbox\Work\toXcel\FARS\rfars\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE5C8BE-F97D-4905-BC00-DB8CD4A9F214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC13C5E-B9EC-4B93-951B-C4F6DF151E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11175" xr2:uid="{F622A617-15FC-4761-9D07-38FE22F3629A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F622A617-15FC-4761-9D07-38FE22F3629A}"/>
   </bookViews>
   <sheets>
     <sheet name="data structure" sheetId="1" r:id="rId1"/>
@@ -638,20 +638,20 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -668,7 +668,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,7 +682,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,7 +696,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -710,7 +710,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -724,7 +724,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -738,7 +738,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -752,7 +752,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -766,7 +766,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,7 +780,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,7 +794,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -808,7 +808,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -825,7 +825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -839,7 +839,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -853,7 +853,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -867,7 +867,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -881,7 +881,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -895,7 +895,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -909,21 +909,21 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="B19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6">
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>3</v>
       </c>
@@ -937,7 +937,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -951,7 +951,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -965,7 +965,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -979,7 +979,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -993,7 +993,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>